<commit_message>
change the bacbone configuration from yaml tasks to jinja2 tepmplate build that being configured using junos_config
</commit_message>
<xml_diff>
--- a/library/network_devices.xlsx
+++ b/library/network_devices.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\infra_new_vlan\library\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD60B96B-D432-4764-8FC8-909B35571ACE}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEF69F9B-B69B-4356-B78B-9D670FC63124}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5505" yWindow="3435" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -572,7 +572,7 @@
   <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
change that all configuration for access and backbone juniper swittches would be done using jinja2 file
</commit_message>
<xml_diff>
--- a/library/network_devices.xlsx
+++ b/library/network_devices.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\infra_new_vlan\library\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEF69F9B-B69B-4356-B78B-9D670FC63124}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB0DAD81-18A8-411B-A75A-976B2DD5838F}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -806,9 +806,14 @@
   </sheetPr>
   <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="52.42578125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">

</xml_diff>

<commit_message>
add support for cisco devices
</commit_message>
<xml_diff>
--- a/library/network_devices.xlsx
+++ b/library/network_devices.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\infra_new_vlan\library\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB0DAD81-18A8-411B-A75A-976B2DD5838F}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89656CED-C8CD-49AE-9FB4-3A53CDEFD078}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="51">
   <si>
     <t>Caption</t>
   </si>
@@ -151,9 +151,6 @@
     <t>PTSW1_Floor7</t>
   </si>
   <si>
-    <t>Type</t>
-  </si>
-  <si>
     <t>junos</t>
   </si>
   <si>
@@ -169,9 +166,6 @@
     <t>qfx</t>
   </si>
   <si>
-    <t>testing</t>
-  </si>
-  <si>
     <t>access</t>
   </si>
   <si>
@@ -179,6 +173,18 @@
   </si>
   <si>
     <t>backbone</t>
+  </si>
+  <si>
+    <t>nexus</t>
+  </si>
+  <si>
+    <t>group</t>
+  </si>
+  <si>
+    <t>none</t>
+  </si>
+  <si>
+    <t>cisco</t>
   </si>
 </sst>
 </file>
@@ -569,16 +575,16 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:I7"/>
+  <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="18.7109375" customWidth="1"/>
     <col min="6" max="6" width="27.5703125" bestFit="1" customWidth="1"/>
@@ -592,16 +598,16 @@
         <v>13</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>30</v>
@@ -621,16 +627,16 @@
         <v>23</v>
       </c>
       <c r="B2" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="C2" t="s">
         <v>31</v>
       </c>
       <c r="D2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="F2" t="s">
         <v>11</v>
@@ -650,16 +656,16 @@
         <v>17</v>
       </c>
       <c r="B3" t="s">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="C3" t="s">
         <v>10</v>
       </c>
       <c r="D3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="F3" t="s">
         <v>32</v>
@@ -679,16 +685,16 @@
         <v>35</v>
       </c>
       <c r="B4" t="s">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="C4" t="s">
         <v>33</v>
       </c>
       <c r="D4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E4" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="F4" t="s">
         <v>32</v>
@@ -708,16 +714,16 @@
         <v>24</v>
       </c>
       <c r="B5" t="s">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="C5" t="s">
         <v>38</v>
       </c>
       <c r="D5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E5" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="F5" t="s">
         <v>11</v>
@@ -737,16 +743,16 @@
         <v>28</v>
       </c>
       <c r="B6" t="s">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="C6" t="s">
         <v>8</v>
       </c>
       <c r="D6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E6" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="F6" t="s">
         <v>11</v>
@@ -766,16 +772,16 @@
         <v>18</v>
       </c>
       <c r="B7" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="C7" t="s">
         <v>14</v>
       </c>
       <c r="D7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E7" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="F7" t="s">
         <v>37</v>
@@ -787,6 +793,35 @@
         <v>2</v>
       </c>
       <c r="I7" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>50</v>
+      </c>
+      <c r="C8" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8" t="s">
+        <v>47</v>
+      </c>
+      <c r="E8" t="s">
+        <v>44</v>
+      </c>
+      <c r="F8" t="s">
+        <v>15</v>
+      </c>
+      <c r="G8" t="s">
+        <v>21</v>
+      </c>
+      <c r="H8" t="s">
+        <v>25</v>
+      </c>
+      <c r="I8" t="s">
         <v>20</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add check to if vlan is a dhcp vlan
</commit_message>
<xml_diff>
--- a/library/network_devices.xlsx
+++ b/library/network_devices.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\infra_new_vlan\library\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0127E9C4-9C13-4397-BA3E-0DE1677D963A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFD1F232-3E5D-4C3C-8699-A6BA1EE0B5F3}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="33600" yWindow="2805" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -711,7 +711,7 @@
   <dimension ref="A1:E26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L17" sqref="L17"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -753,7 +753,7 @@
         <v>19</v>
       </c>
       <c r="E2" s="15" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -829,7 +829,7 @@
         <v>8</v>
       </c>
       <c r="B7" s="14" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="C7" s="14" t="s">
         <v>5</v>
@@ -846,7 +846,7 @@
         <v>1</v>
       </c>
       <c r="B8" s="14" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C8" s="14" t="s">
         <v>6</v>

</xml_diff>